<commit_message>
Poprawka niejednoznaczności w przypisaniu zadań
</commit_message>
<xml_diff>
--- a/doc/template_MK.xlsx
+++ b/doc/template_MK.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="APSY" sheetId="1" state="visible" r:id="rId2"/>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Kompetencje twarde dla Serwisu</t>
   </si>
   <si>
-    <t xml:space="preserve">st1,st2,st3,st4,st5,st7,st8,st8,st9,st10</t>
+    <t xml:space="preserve">st1,st2,st3,st4,st5,st6,st7,st8,st9,st10,st11</t>
   </si>
   <si>
     <t xml:space="preserve">unikalny identyfikator zadania (tylko małe litery i cyfry, bez spacji)</t>
@@ -3633,8 +3633,8 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3696,8 +3696,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3849,8 +3849,8 @@
   </sheetPr>
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A81" activeCellId="0" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6412,6 +6412,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="18.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="64.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>